<commit_message>
Built site for kwb.impetus: 0.0.0.9000@8cf6c78
</commit_message>
<xml_diff>
--- a/impetus_flows_v1.0.0.xlsx
+++ b/impetus_flows_v1.0.0.xlsx
@@ -694,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>50338159.103417</v>
+        <v>50338157.6716721</v>
       </c>
     </row>
     <row r="5">
@@ -702,7 +702,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>39012073.3051482</v>
+        <v>39012072.1955459</v>
       </c>
     </row>
     <row r="6">
@@ -710,7 +710,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>31331008.4891758</v>
+        <v>31331007.5980424</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Built site for kwb.impetus: 0.0.0.9000@c6931a1
</commit_message>
<xml_diff>
--- a/impetus_flows_v1.0.0.xlsx
+++ b/impetus_flows_v1.0.0.xlsx
@@ -694,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>50338157.6716721</v>
+        <v>50338729.409502</v>
       </c>
     </row>
     <row r="5">
@@ -702,7 +702,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>39012072.1955459</v>
+        <v>39012515.2923641</v>
       </c>
     </row>
     <row r="6">
@@ -710,7 +710,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>31331007.5980424</v>
+        <v>31331363.4537813</v>
       </c>
     </row>
     <row r="7">

</xml_diff>